<commit_message>
Observaciones a los datos de Mario
</commit_message>
<xml_diff>
--- a/Proyectos/Mario_BisecciónTemporal/Signal Detection Theory Agosto_2017.xlsx
+++ b/Proyectos/Mario_BisecciónTemporal/Signal Detection Theory Agosto_2017.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nueva carpeta (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Proyectos\Mario_BisecciónTemporal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -384,7 +384,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -622,7 +622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -954,6 +954,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -992,7 +993,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1053,7 +1054,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1114,7 +1115,7 @@
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1175,7 +1176,7 @@
         <xdr:cNvPr id="5" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1236,7 +1237,7 @@
         <xdr:cNvPr id="6" name="Imagen 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1297,7 +1298,7 @@
         <xdr:cNvPr id="7" name="Imagen 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1358,7 +1359,7 @@
         <xdr:cNvPr id="8" name="Imagen 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1419,7 +1420,7 @@
         <xdr:cNvPr id="9" name="Imagen 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1460,6 +1461,92 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1206500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1063625</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="CuadroTexto 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1603375" y="6445250"/>
+          <a:ext cx="6381750" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="2800"/>
+            <a:t>FA 1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-MX" sz="2800" baseline="0"/>
+            <a:t> por como está definido son Rechazos correctos</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-MX" sz="2800" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="2800" baseline="0"/>
+            <a:t>Ensayos con Señal = Hits + Omisiones</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-MX" sz="2800" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="2800" baseline="0"/>
+            <a:t>Ensayos con Ruido = FA + Rechazos correctos</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1731,7 +1818,7 @@
   <dimension ref="B1:AH88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4266,8 +4353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AH88"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5237,34 +5324,34 @@
       <c r="G30" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="119">
         <v>43</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30" s="119">
         <v>28</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30" s="119">
         <v>23</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30" s="119">
         <v>34</v>
       </c>
-      <c r="L30" s="1">
+      <c r="L30" s="119">
         <v>42</v>
       </c>
-      <c r="M30" s="1">
+      <c r="M30" s="119">
         <v>32</v>
       </c>
-      <c r="N30" s="1">
+      <c r="N30" s="119">
         <v>34</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O30" s="119">
         <v>33</v>
       </c>
-      <c r="P30" s="1">
+      <c r="P30" s="119">
         <v>34</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="Q30" s="119">
         <v>31</v>
       </c>
     </row>
@@ -5319,34 +5406,34 @@
       <c r="G32" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32" s="119">
         <v>34</v>
       </c>
-      <c r="I32" s="1">
+      <c r="I32" s="119">
         <v>36</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J32" s="119">
         <v>32</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K32" s="119">
         <v>31</v>
       </c>
-      <c r="L32" s="1">
+      <c r="L32" s="119">
         <v>41</v>
       </c>
-      <c r="M32" s="1">
+      <c r="M32" s="119">
         <v>39</v>
       </c>
-      <c r="N32" s="1">
+      <c r="N32" s="119">
         <v>32</v>
       </c>
-      <c r="O32" s="1">
+      <c r="O32" s="119">
         <v>26</v>
       </c>
-      <c r="P32" s="1">
+      <c r="P32" s="119">
         <v>38</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="Q32" s="119">
         <v>25</v>
       </c>
     </row>

</xml_diff>